<commit_message>
Date changes in sprint Plan
</commit_message>
<xml_diff>
--- a/sprintplan.xlsx
+++ b/sprintplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\lockers-lockedme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7D08141-CC41-4E39-AA9E-07033ABCFE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDECD0F-0E1F-47AF-BE68-88BC2D3B0CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E50A6177-47FE-4283-9C4E-1BDEFD6A7733}"/>
   </bookViews>
@@ -129,7 +129,7 @@
     <t>Submit Project</t>
   </si>
   <si>
-    <t>Retest Application</t>
+    <t>Regression Test</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +872,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="4">
-        <v>44624</v>
+        <v>44648</v>
       </c>
       <c r="E16" s="4">
         <v>37351</v>
@@ -892,7 +892,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="4">
-        <v>44625</v>
+        <v>44648</v>
       </c>
       <c r="E17" s="4">
         <v>37352</v>
@@ -912,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="4">
-        <v>44625</v>
+        <v>44648</v>
       </c>
       <c r="E18" s="4">
         <v>37352</v>
@@ -932,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="4">
-        <v>44625</v>
+        <v>44641</v>
       </c>
       <c r="E19" s="4">
         <v>37352</v>

</xml_diff>